<commit_message>
ANEXO DE DOCUMENTO MANUAL SOPORTE
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="105">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -375,6 +375,9 @@
   </si>
   <si>
     <t>Transferencias deposito virtual Pachuco</t>
+  </si>
+  <si>
+    <t>Manual de politicas de Tecnologia de la Informacion de la DGT-CCFN</t>
   </si>
 </sst>
 </file>
@@ -527,30 +530,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -565,11 +544,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1228,7 +1231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -1243,36 +1246,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1282,13 +1285,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1297,13 +1300,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1312,13 +1315,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1327,13 +1330,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1342,13 +1345,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1357,13 +1360,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1372,13 +1375,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1387,37 +1390,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1426,97 +1429,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1525,25 +1528,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1552,25 +1555,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1579,13 +1582,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1594,13 +1597,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1609,13 +1612,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1624,61 +1627,61 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1688,132 +1691,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1830,26 +1834,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1878,36 +1881,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1917,317 +1920,317 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2237,111 +2240,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2355,48 +2400,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2410,8 +2413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,36 +2427,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2463,313 +2466,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="C8" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2779,111 +2784,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2897,48 +2944,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2967,36 +2972,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3006,13 +3011,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3021,13 +3026,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3036,13 +3041,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3051,13 +3056,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3066,13 +3071,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3081,13 +3086,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3096,13 +3101,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3111,13 +3116,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3126,13 +3131,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3141,227 +3146,227 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3371,111 +3376,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3489,48 +3536,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
INGRESO DE FORMATO ORDEN DE COMPRA
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="106">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Manual de politicas de Tecnologia de la Informacion de la DGT-CCFN</t>
+  </si>
+  <si>
+    <t>Orden de compra</t>
   </si>
 </sst>
 </file>
@@ -530,6 +533,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -544,35 +571,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1246,36 +1249,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1285,13 +1288,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1300,13 +1303,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1315,13 +1318,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1330,13 +1333,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1345,13 +1348,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1360,13 +1363,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1375,13 +1378,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1390,37 +1393,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1429,97 +1432,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1528,25 +1531,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1555,25 +1558,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1582,13 +1585,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1597,13 +1600,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1612,13 +1615,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1627,61 +1630,61 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1691,133 +1694,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1834,25 +1836,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1881,36 +1884,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1920,317 +1923,317 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2240,153 +2243,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2400,6 +2361,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2413,7 +2416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -2427,36 +2430,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2466,315 +2469,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2784,153 +2787,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2944,6 +2905,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2957,8 +2960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,36 +2975,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3011,13 +3014,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3026,13 +3029,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3041,13 +3044,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3056,13 +3059,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3071,13 +3074,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3086,13 +3089,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3101,13 +3104,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3116,13 +3119,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3131,13 +3134,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3146,227 +3149,229 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3376,111 +3381,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3494,48 +3541,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
MANUAL DESCARGA DE FACTURAS
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -381,6 +381,9 @@
   </si>
   <si>
     <t>Orden de compra</t>
+  </si>
+  <si>
+    <t>Manual de usuario Descarga de facturas</t>
   </si>
 </sst>
 </file>
@@ -533,30 +536,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -571,11 +550,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1249,36 +1252,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1288,13 +1291,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1303,13 +1306,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1318,13 +1321,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1333,13 +1336,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1348,13 +1351,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1363,13 +1366,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1378,13 +1381,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1393,37 +1396,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1432,97 +1435,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1531,25 +1534,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1558,25 +1561,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1585,13 +1588,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1600,13 +1603,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1615,13 +1618,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1630,61 +1633,61 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1694,132 +1697,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1836,26 +1840,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1870,7 +1873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10:G10"/>
     </sheetView>
   </sheetViews>
@@ -1884,36 +1887,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1923,317 +1926,319 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2243,111 +2248,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2361,48 +2408,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2430,36 +2435,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2469,315 +2474,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2787,111 +2792,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2905,48 +2952,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2960,7 +2965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -2975,36 +2980,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3014,13 +3019,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3029,13 +3034,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3044,13 +3049,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3059,13 +3064,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3074,13 +3079,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3089,13 +3094,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3104,13 +3109,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3119,13 +3124,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3134,13 +3139,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3149,229 +3154,229 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3381,111 +3386,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3499,48 +3546,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FORMATO ALTA/BAJA DE USUARIOS
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="109">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>manual de usuario Descarga de facturas para administrador</t>
+  </si>
+  <si>
+    <t>Formato Alta/Baja de Usuarios</t>
   </si>
 </sst>
 </file>
@@ -539,30 +542,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -577,11 +556,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1255,36 +1258,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1294,13 +1297,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1309,13 +1312,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1324,13 +1327,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1339,13 +1342,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1354,13 +1357,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1369,13 +1372,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1384,13 +1387,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1399,37 +1402,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1438,97 +1441,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1537,25 +1540,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1564,25 +1567,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1591,13 +1594,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1606,13 +1609,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1621,13 +1624,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1636,61 +1639,61 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1700,132 +1703,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1842,26 +1846,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1876,7 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:G11"/>
     </sheetView>
   </sheetViews>
@@ -1890,36 +1893,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1929,321 +1932,321 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2253,111 +2256,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2371,48 +2416,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2440,36 +2443,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2479,315 +2482,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2797,111 +2800,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2915,48 +2960,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2970,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,36 +2988,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3024,13 +3027,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3039,13 +3042,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3054,13 +3057,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3069,13 +3072,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3084,13 +3087,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3099,13 +3102,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3114,13 +3117,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3129,13 +3132,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3144,13 +3147,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3159,229 +3162,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3391,111 +3396,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3509,48 +3556,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
PROYECTO CONTROL DE VENTAS DE PLATILLOS EN COCINA
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="109">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -383,13 +383,13 @@
     <t>Orden de compra</t>
   </si>
   <si>
-    <t>Manual de usuario Descarga de facturas para cliente</t>
-  </si>
-  <si>
-    <t>manual de usuario Descarga de facturas para administrador</t>
-  </si>
-  <si>
     <t>Formato Alta/Baja de Usuarios</t>
+  </si>
+  <si>
+    <t>Control de ventas de platillos en cocina</t>
+  </si>
+  <si>
+    <t>CCFN Descarga de Facturas</t>
   </si>
 </sst>
 </file>
@@ -542,6 +542,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -556,35 +580,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,36 +1258,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1297,13 +1297,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1312,13 +1312,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1327,13 +1327,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1342,13 +1342,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1357,13 +1357,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1372,13 +1372,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1387,13 +1387,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1402,37 +1402,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1441,97 +1441,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1540,25 +1540,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1567,25 +1567,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1594,13 +1594,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1609,13 +1609,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1624,13 +1624,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1639,61 +1639,68 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1703,133 +1710,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1846,25 +1852,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1880,7 +1887,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:G11"/>
+      <selection activeCell="C15" sqref="C15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,36 +1900,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1932,321 +1939,317 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2256,153 +2259,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2416,6 +2377,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2443,36 +2446,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2482,315 +2485,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2800,153 +2803,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2960,6 +2921,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2973,7 +2976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
@@ -2988,36 +2991,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3027,13 +3030,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3042,13 +3045,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3057,13 +3060,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3072,13 +3075,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3087,13 +3090,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3102,13 +3105,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3117,13 +3120,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3132,13 +3135,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3147,13 +3150,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3162,231 +3165,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3396,111 +3399,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3514,48 +3559,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Proyecto CCFN Descarga de facturas
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -390,6 +390,15 @@
   </si>
   <si>
     <t>CCFN Descarga de Facturas</t>
+  </si>
+  <si>
+    <t>CCFN Descarga de facturas</t>
+  </si>
+  <si>
+    <t>CCFN Descarga de facturas Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberacion de IP </t>
   </si>
 </sst>
 </file>
@@ -542,30 +551,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -580,11 +565,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1243,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:G34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,36 +1267,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1297,13 +1306,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1312,13 +1321,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1327,13 +1336,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1342,13 +1351,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1357,13 +1366,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1372,13 +1381,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1387,13 +1396,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1402,37 +1411,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1441,97 +1450,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1540,25 +1549,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1567,25 +1576,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1594,13 +1603,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1609,13 +1618,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1624,13 +1633,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1639,13 +1648,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1654,53 +1663,53 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1710,132 +1719,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1852,26 +1862,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1887,7 +1896,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:G15"/>
+      <selection activeCell="C14" sqref="C14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1900,36 +1909,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1939,317 +1948,323 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2259,111 +2274,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2377,48 +2434,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2446,36 +2461,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2485,315 +2500,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2803,111 +2818,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2921,48 +2978,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2991,36 +3006,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3030,13 +3045,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3045,13 +3060,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3060,13 +3075,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3075,13 +3090,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3090,13 +3105,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3105,13 +3120,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3120,13 +3135,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3135,13 +3150,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3150,13 +3165,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3165,231 +3180,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3399,111 +3414,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3517,48 +3574,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
MANUAL DE CAMBIO DE MONEDA
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="113">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t xml:space="preserve">Liberacion de IP </t>
+  </si>
+  <si>
+    <t>Cambio de Moneda</t>
   </si>
 </sst>
 </file>
@@ -551,6 +554,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -565,35 +592,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1252,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -1267,36 +1270,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1306,13 +1309,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1321,13 +1324,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1336,13 +1339,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1351,13 +1354,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1366,13 +1369,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1381,13 +1384,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1396,13 +1399,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1411,37 +1414,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1450,97 +1453,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1549,25 +1552,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1576,25 +1579,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1603,13 +1606,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1618,13 +1621,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1633,13 +1636,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1648,13 +1651,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1663,53 +1666,53 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1719,133 +1722,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1862,25 +1864,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1895,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,36 +1912,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1948,323 +1951,325 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2274,153 +2279,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2434,6 +2397,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2461,36 +2466,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2500,315 +2505,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2818,153 +2823,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2978,6 +2941,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3006,36 +3011,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3045,13 +3050,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3060,13 +3065,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3075,13 +3080,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3090,13 +3095,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3105,13 +3110,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3120,13 +3125,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3135,13 +3140,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3150,13 +3155,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3165,13 +3170,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3180,231 +3185,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3414,111 +3419,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3532,48 +3579,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual de transferencia de salida y entrada.
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="115">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -402,6 +402,12 @@
   </si>
   <si>
     <t>Cambio de Moneda</t>
+  </si>
+  <si>
+    <t>Transferencia salida</t>
+  </si>
+  <si>
+    <t>Transferencia entrada</t>
   </si>
 </sst>
 </file>
@@ -554,30 +560,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -592,11 +574,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1270,36 +1276,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1309,13 +1315,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1324,13 +1330,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1339,13 +1345,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1354,13 +1360,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1369,13 +1375,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1384,13 +1390,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1399,13 +1405,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1414,37 +1420,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1453,97 +1459,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1552,25 +1558,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1579,25 +1585,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1606,13 +1612,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1621,13 +1627,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1636,13 +1642,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1651,13 +1657,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1666,53 +1672,53 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1722,132 +1728,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1864,26 +1871,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1899,7 +1905,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:G15"/>
+      <selection activeCell="C14" sqref="C14:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,36 +1918,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1951,325 +1957,329 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2279,111 +2289,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2397,48 +2449,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2466,36 +2476,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2505,315 +2515,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2823,111 +2833,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2941,48 +2993,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3011,36 +3021,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3050,13 +3060,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3065,13 +3075,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3080,13 +3090,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3095,13 +3105,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3110,13 +3120,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3125,13 +3135,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3140,13 +3150,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3155,13 +3165,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3170,13 +3180,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3185,231 +3195,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3419,111 +3429,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3537,48 +3589,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Guia para impresion de planilla
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="116">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>Transferencia entrada</t>
+  </si>
+  <si>
+    <t>Guia para impresion de planilla.</t>
   </si>
 </sst>
 </file>
@@ -560,6 +563,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -574,35 +601,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1276,36 +1279,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1315,13 +1318,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1330,13 +1333,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1345,13 +1348,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1360,13 +1363,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1375,13 +1378,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1390,13 +1393,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1405,13 +1408,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1420,37 +1423,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1459,97 +1462,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1558,25 +1561,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1585,25 +1588,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1612,13 +1615,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1627,13 +1630,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1642,13 +1645,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1657,13 +1660,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1672,53 +1675,53 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1728,133 +1731,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1871,25 +1873,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1905,7 +1908,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:G14"/>
+      <selection activeCell="C17" sqref="C17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,36 +1921,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1957,329 +1960,331 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2289,153 +2294,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2449,6 +2412,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2476,36 +2481,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2515,315 +2520,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2833,153 +2838,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2993,6 +2956,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3021,36 +3026,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3060,13 +3065,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3075,13 +3080,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3090,13 +3095,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3105,13 +3110,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3120,13 +3125,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3135,13 +3140,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3150,13 +3155,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3165,13 +3170,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3180,13 +3185,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3195,231 +3200,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3429,111 +3434,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3547,48 +3594,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ingreso de proyecto de comisiones
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="119">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -411,6 +411,15 @@
   </si>
   <si>
     <t>Guia para impresion de planilla.</t>
+  </si>
+  <si>
+    <t>Aldo</t>
+  </si>
+  <si>
+    <t>Comisiones por producto a vendedores.</t>
+  </si>
+  <si>
+    <t>Rafael.</t>
   </si>
 </sst>
 </file>
@@ -563,30 +572,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -601,11 +586,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1264,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,36 +1288,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1318,13 +1327,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1333,13 +1342,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1348,13 +1357,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1363,13 +1372,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1378,13 +1387,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1393,13 +1402,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1408,13 +1417,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1423,37 +1432,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1462,97 +1471,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1561,25 +1570,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1588,25 +1597,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1615,13 +1624,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1630,13 +1639,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1645,13 +1654,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1660,203 +1669,212 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+    <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
-    </row>
-    <row r="42" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="G41" s="23"/>
+    </row>
+    <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="G43" s="24"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="G44" s="24"/>
+    </row>
+    <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+    </row>
+    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1873,26 +1891,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1907,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,36 +1938,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1960,331 +1977,331 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2294,111 +2311,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2412,48 +2471,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2481,36 +2498,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2520,315 +2537,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2838,111 +2855,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2956,48 +3015,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3026,36 +3043,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3065,13 +3082,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3080,13 +3097,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3095,13 +3112,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3110,13 +3127,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3125,13 +3142,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3140,13 +3157,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3155,13 +3172,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3170,13 +3187,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3185,13 +3202,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3200,231 +3217,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3434,111 +3451,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3552,48 +3611,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ingreso de manual para respaldar BD en sistema de nomina
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="120">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>Rafael.</t>
+  </si>
+  <si>
+    <t>Manual para respaldar BD en sistema de nomina TRESS</t>
   </si>
 </sst>
 </file>
@@ -572,6 +575,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -586,35 +613,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1273,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -1288,36 +1291,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1327,13 +1330,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1342,13 +1345,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1357,13 +1360,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1372,13 +1375,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1387,13 +1390,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1402,13 +1405,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1417,13 +1420,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1432,37 +1435,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1471,97 +1474,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1570,25 +1573,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1597,25 +1600,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1624,13 +1627,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1639,13 +1642,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1654,13 +1657,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1669,13 +1672,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1684,13 +1687,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1699,13 +1702,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1714,31 +1717,31 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1748,133 +1751,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1891,25 +1893,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1924,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,36 +1941,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1977,331 +1980,333 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2311,153 +2316,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2471,6 +2434,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2498,36 +2503,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2537,315 +2542,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2855,153 +2860,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3015,6 +2978,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3043,36 +3048,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3082,13 +3087,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3097,13 +3102,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3112,13 +3117,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3127,13 +3132,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3142,13 +3147,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3157,13 +3162,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3172,13 +3177,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3187,13 +3192,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3202,13 +3207,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3217,231 +3222,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3451,111 +3456,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3569,48 +3616,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual de usuario instalacion Tress
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="121">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>Manual para respaldar BD en sistema de nomina TRESS</t>
+  </si>
+  <si>
+    <t>Instalacion de Sistema Tress</t>
   </si>
 </sst>
 </file>
@@ -575,30 +578,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -613,11 +592,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1291,36 +1294,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1330,13 +1333,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1345,13 +1348,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1360,13 +1363,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1375,13 +1378,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1390,13 +1393,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1405,13 +1408,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1420,13 +1423,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1435,37 +1438,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1474,97 +1477,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1573,25 +1576,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1600,25 +1603,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1627,13 +1630,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1642,13 +1645,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1657,13 +1660,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1672,13 +1675,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1687,13 +1690,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1702,13 +1705,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1717,31 +1720,31 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1751,132 +1754,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1893,26 +1897,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1928,7 +1931,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C20:G21"/>
+      <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,36 +1944,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1980,333 +1983,335 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2316,111 +2321,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2434,48 +2481,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2503,36 +2508,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2542,315 +2547,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2860,111 +2865,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2978,48 +3025,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3048,36 +3053,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3087,13 +3092,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3102,13 +3107,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3117,13 +3122,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3132,13 +3137,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3147,13 +3152,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3162,13 +3167,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3177,13 +3182,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3192,13 +3197,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3207,13 +3212,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3222,231 +3227,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3456,111 +3461,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3574,48 +3621,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Transferencia de UUID a polizas
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="122">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>Instalacion de Sistema Tress</t>
+  </si>
+  <si>
+    <t>Traslado de UUID a polizas</t>
   </si>
 </sst>
 </file>
@@ -578,6 +581,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -592,35 +619,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1279,51 +1282,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1333,13 +1336,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1348,13 +1351,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1363,13 +1366,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1378,13 +1381,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1393,13 +1396,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1408,13 +1411,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1423,13 +1426,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1438,37 +1441,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1477,97 +1480,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1576,25 +1579,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1603,25 +1606,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1630,13 +1633,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1645,13 +1648,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1660,13 +1663,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1675,13 +1678,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1690,13 +1693,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1705,13 +1708,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1720,31 +1723,36 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1754,133 +1762,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1897,25 +1904,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1930,7 +1938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18:G18"/>
     </sheetView>
   </sheetViews>
@@ -1944,36 +1952,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1983,335 +1991,335 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2321,153 +2329,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2481,6 +2447,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2508,36 +2516,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2547,315 +2555,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2865,153 +2873,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3025,6 +2991,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3053,36 +3061,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3092,13 +3100,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3107,13 +3115,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3122,13 +3130,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3137,13 +3145,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3152,13 +3160,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3167,13 +3175,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3182,13 +3190,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3197,13 +3205,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3212,13 +3220,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3227,231 +3235,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3461,111 +3469,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3579,48 +3629,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual de usuario Lista de surtido para almcacenes y sucursales mayoreo
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="123">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>Traslado de UUID a polizas</t>
+  </si>
+  <si>
+    <t>Lista de surtido para almacenes y sucursales mayoreo.</t>
   </si>
 </sst>
 </file>
@@ -581,30 +584,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -619,11 +598,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1282,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C27" sqref="C27:G27"/>
     </sheetView>
   </sheetViews>
@@ -1297,36 +1300,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1336,13 +1339,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1351,13 +1354,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1366,13 +1369,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1381,13 +1384,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1396,13 +1399,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1411,13 +1414,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1426,13 +1429,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1441,37 +1444,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1480,97 +1483,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1579,25 +1582,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1606,25 +1609,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1633,13 +1636,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1648,13 +1651,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1663,13 +1666,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1678,13 +1681,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1693,13 +1696,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1708,13 +1711,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1723,13 +1726,13 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
       <c r="H35" t="s">
         <v>93</v>
       </c>
@@ -1738,21 +1741,21 @@
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1762,132 +1765,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1904,26 +1908,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1938,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,36 +1955,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1991,335 +1994,337 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2329,111 +2334,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2447,48 +2494,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2516,36 +2521,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2555,315 +2560,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2873,111 +2878,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2991,48 +3038,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3061,36 +3066,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3100,13 +3105,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3115,13 +3120,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3130,13 +3135,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3145,13 +3150,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3160,13 +3165,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3175,13 +3180,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3190,13 +3195,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3205,13 +3210,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3220,13 +3225,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3235,231 +3240,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3469,111 +3474,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3587,48 +3634,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manual de usuario Lista de surtdo para almacenes y sucursales mayoreo
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -431,7 +431,7 @@
     <t>Traslado de UUID a polizas</t>
   </si>
   <si>
-    <t>Lista de surtido para almacenes y sucursales mayoreo.</t>
+    <t>Lista de surtido para almacenes y sucursales mayoreo</t>
   </si>
 </sst>
 </file>
@@ -584,6 +584,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -598,35 +622,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1300,36 +1300,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1339,13 +1339,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1354,13 +1354,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1369,13 +1369,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1384,13 +1384,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1399,13 +1399,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1414,13 +1414,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1429,13 +1429,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1444,37 +1444,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1483,97 +1483,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1582,25 +1582,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1609,25 +1609,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1636,13 +1636,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1651,13 +1651,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1666,13 +1666,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1681,13 +1681,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1696,13 +1696,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1711,13 +1711,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1726,13 +1726,13 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
       <c r="H35" t="s">
         <v>93</v>
       </c>
@@ -1741,21 +1741,21 @@
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1765,133 +1765,132 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1908,25 +1907,26 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1941,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:G19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,36 +1955,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1994,337 +1994,337 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2334,153 +2334,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2494,6 +2452,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2521,36 +2521,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2560,315 +2560,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2878,153 +2878,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3038,6 +2996,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3066,36 +3066,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3105,13 +3105,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3120,13 +3120,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3135,13 +3135,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3150,13 +3150,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3165,13 +3165,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3180,13 +3180,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3195,13 +3195,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3210,13 +3210,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3225,13 +3225,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3240,231 +3240,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3474,111 +3474,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3592,48 +3634,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Status CFDI activacion WF no timbrados
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="124">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>Lista de surtido para almacenes y sucursales mayoreo</t>
+  </si>
+  <si>
+    <t>Status CFDI activacion WF no timbrados.</t>
   </si>
 </sst>
 </file>
@@ -584,30 +587,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -622,11 +601,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1300,36 +1303,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1339,13 +1342,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1354,13 +1357,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1369,13 +1372,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1384,13 +1387,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1399,13 +1402,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1414,13 +1417,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1429,13 +1432,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1444,37 +1447,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1483,97 +1486,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1582,25 +1585,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1609,25 +1612,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1636,13 +1639,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1651,13 +1654,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1666,13 +1669,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1681,13 +1684,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1696,13 +1699,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1711,13 +1714,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1726,13 +1729,13 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
       <c r="H35" t="s">
         <v>93</v>
       </c>
@@ -1741,21 +1744,21 @@
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -1765,132 +1768,133 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
@@ -1907,26 +1911,25 @@
     <mergeCell ref="F41:G41"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1942,7 +1945,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:G21"/>
+      <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,36 +1958,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1994,337 +1997,339 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2334,111 +2339,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2452,48 +2499,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2521,36 +2526,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2560,315 +2565,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2878,111 +2883,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2996,48 +3043,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3066,36 +3071,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="22"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3105,13 +3110,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3120,13 +3125,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3135,13 +3140,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3150,13 +3155,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3165,13 +3170,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3180,13 +3185,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3195,13 +3200,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3210,13 +3215,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3225,13 +3230,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3240,231 +3245,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3474,111 +3479,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21" t="s">
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="23"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="19"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15" t="s">
+      <c r="E43" s="24"/>
+      <c r="F43" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="15"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="24"/>
+      <c r="D44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15" t="s">
+      <c r="E44" s="24"/>
+      <c r="F44" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="15"/>
+      <c r="G44" s="24"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="26"/>
+      <c r="E48" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="27"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3592,48 +3639,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Proceso de cobro de facturas en cyc
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="136">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -435,6 +435,42 @@
   </si>
   <si>
     <t>Status CFDI activacion WF no timbrados.</t>
+  </si>
+  <si>
+    <t>Proceso de cobro de facturas en cyc</t>
+  </si>
+  <si>
+    <t>joaquin</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>039</t>
+  </si>
+  <si>
+    <t>040</t>
   </si>
 </sst>
 </file>
@@ -560,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -587,6 +623,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -601,38 +661,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1286,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H50"/>
+  <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,36 +1342,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1342,13 +1381,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1357,13 +1396,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>91</v>
       </c>
@@ -1372,13 +1411,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>94</v>
       </c>
@@ -1387,13 +1426,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>93</v>
       </c>
@@ -1402,13 +1441,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>93</v>
       </c>
@@ -1417,13 +1456,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>91</v>
       </c>
@@ -1432,13 +1471,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>94</v>
       </c>
@@ -1447,37 +1486,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" t="s">
         <v>95</v>
       </c>
@@ -1486,97 +1525,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
       <c r="H24" t="s">
         <v>96</v>
       </c>
@@ -1585,25 +1624,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
       <c r="H26" t="s">
         <v>93</v>
       </c>
@@ -1612,25 +1651,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
       <c r="H28" t="s">
         <v>94</v>
       </c>
@@ -1639,13 +1678,13 @@
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
       <c r="H29" t="s">
         <v>94</v>
       </c>
@@ -1654,13 +1693,13 @@
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
       <c r="H30" t="s">
         <v>93</v>
       </c>
@@ -1669,13 +1708,13 @@
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
       <c r="H31" t="s">
         <v>94</v>
       </c>
@@ -1684,13 +1723,13 @@
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
       <c r="H32" t="s">
         <v>94</v>
       </c>
@@ -1699,13 +1738,13 @@
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
       <c r="H33" t="s">
         <v>116</v>
       </c>
@@ -1714,13 +1753,13 @@
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
       <c r="H34" t="s">
         <v>118</v>
       </c>
@@ -1729,13 +1768,13 @@
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
       <c r="H35" t="s">
         <v>93</v>
       </c>
@@ -1744,173 +1783,260 @@
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="40" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B38" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="29"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C51" s="21"/>
+      <c r="D51" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E51" s="21"/>
+      <c r="F51" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
-    </row>
-    <row r="42" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="E52" s="19"/>
+      <c r="F52" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C53" s="15"/>
+      <c r="D53" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E53" s="15"/>
+      <c r="F53" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="G53" s="15"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C54" s="15"/>
+      <c r="D54" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E54" s="15"/>
+      <c r="F54" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
-    </row>
-    <row r="47" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="G54" s="15"/>
+    </row>
+    <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-    </row>
-    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="6" t="s">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+    </row>
+    <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C58" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D58" s="17"/>
+      <c r="E58" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="7"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="7"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
+  <mergeCells count="65">
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="C21:G21"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C11:G11"/>
@@ -1923,18 +2049,47 @@
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B8:B24 B25:B26 B27:B28 B29:B37" numberStoredAsText="1"/>
+    <ignoredError sqref="B8:B24 B25:B26 B27:B28 B29:B37 B38:B47" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -1944,7 +2099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
@@ -1958,36 +2113,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1997,339 +2152,339 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2339,153 +2494,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2499,6 +2612,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2526,36 +2681,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="28" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2565,315 +2720,315 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2883,153 +3038,111 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3043,6 +3156,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3071,36 +3226,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3110,13 +3265,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3125,13 +3280,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="H8" t="s">
         <v>88</v>
       </c>
@@ -3140,13 +3295,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="H9" t="s">
         <v>88</v>
       </c>
@@ -3155,13 +3310,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" t="s">
         <v>88</v>
       </c>
@@ -3170,13 +3325,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" t="s">
         <v>88</v>
       </c>
@@ -3185,13 +3340,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
       <c r="H12" t="s">
         <v>89</v>
       </c>
@@ -3200,13 +3355,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -3215,13 +3370,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
       <c r="H14" t="s">
         <v>88</v>
       </c>
@@ -3230,13 +3385,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
       <c r="H15" t="s">
         <v>88</v>
       </c>
@@ -3245,231 +3400,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3479,111 +3634,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="23" t="s">
+      <c r="B41" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="23"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24" t="s">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24" t="s">
+      <c r="E43" s="15"/>
+      <c r="F43" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="24"/>
+      <c r="G43" s="15"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24" t="s">
+      <c r="E44" s="15"/>
+      <c r="F44" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="24"/>
+      <c r="G44" s="15"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27" t="s">
+      <c r="D48" s="17"/>
+      <c r="E48" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3597,48 +3794,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Consulta historial de impresiones y movimientos
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="138">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t>Proceso de cobro de facturas en CyC</t>
+  </si>
+  <si>
+    <t>Entrada de facturas para Sistemas</t>
+  </si>
+  <si>
+    <t>Consulta historial de impresiones y movimientos</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1334,7 @@
   <dimension ref="B1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:G36"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,11 +1804,16 @@
       <c r="B37" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="14"/>
+      <c r="C37" s="14" t="s">
+        <v>137</v>
+      </c>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
+      <c r="H37" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
@@ -2099,8 +2110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:G20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,7 +2331,9 @@
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>

</xml_diff>

<commit_message>
MANUAL DE USUARIO GENERACION DE NOTAS DE CREDITO
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="139">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>Consulta historial de impresiones y movimientos</t>
+  </si>
+  <si>
+    <t>Generacion de Notas de Credito.</t>
   </si>
 </sst>
 </file>
@@ -637,6 +640,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,27 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1333,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -1348,32 +1351,32 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1387,13 +1390,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1924,94 +1927,94 @@
       <c r="G48" s="8"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="23" t="s">
+      <c r="B50" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24" t="s">
+      <c r="C51" s="22"/>
+      <c r="D51" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24" t="s">
+      <c r="E51" s="22"/>
+      <c r="F51" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="24"/>
+      <c r="G51" s="22"/>
     </row>
     <row r="52" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22" t="s">
+      <c r="C52" s="20"/>
+      <c r="D52" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22" t="s">
+      <c r="E52" s="20"/>
+      <c r="F52" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="22"/>
+      <c r="G52" s="20"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25" t="s">
+      <c r="C53" s="16"/>
+      <c r="D53" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25" t="s">
+      <c r="E53" s="16"/>
+      <c r="F53" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="25"/>
+      <c r="G53" s="16"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25" t="s">
+      <c r="C54" s="16"/>
+      <c r="D54" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25" t="s">
+      <c r="E54" s="16"/>
+      <c r="F54" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G54" s="25"/>
+      <c r="G54" s="16"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
     </row>
     <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="27" t="s">
+      <c r="C58" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D58" s="27"/>
-      <c r="E58" s="28" t="s">
+      <c r="D58" s="18"/>
+      <c r="E58" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
@@ -2031,26 +2034,35 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
@@ -2067,35 +2079,26 @@
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2110,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:G24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,29 +2127,29 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="29" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
-      <c r="F3" s="21"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -2163,13 +2166,13 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -2343,7 +2346,9 @@
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
@@ -2507,92 +2512,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24" t="s">
+      <c r="C41" s="22"/>
+      <c r="D41" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24" t="s">
+      <c r="E41" s="22"/>
+      <c r="F41" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="24"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22" t="s">
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="22"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="25"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25" t="s">
+      <c r="E44" s="16"/>
+      <c r="F44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="25"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="28" t="s">
+      <c r="D48" s="18"/>
+      <c r="E48" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -2612,48 +2617,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2667,6 +2630,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2694,29 +2699,29 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="29" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
-      <c r="F3" s="21"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -2733,13 +2738,13 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -3051,92 +3056,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24" t="s">
+      <c r="C41" s="22"/>
+      <c r="D41" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24" t="s">
+      <c r="E41" s="22"/>
+      <c r="F41" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="24"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22" t="s">
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="22"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="25"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25" t="s">
+      <c r="E44" s="16"/>
+      <c r="F44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="25"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="28" t="s">
+      <c r="D48" s="18"/>
+      <c r="E48" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -3156,48 +3161,6 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3211,6 +3174,48 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3239,32 +3244,32 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="18"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
@@ -3278,13 +3283,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3647,92 +3652,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+      <c r="B40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24" t="s">
+      <c r="C41" s="22"/>
+      <c r="D41" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24" t="s">
+      <c r="E41" s="22"/>
+      <c r="F41" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="24"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22" t="s">
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="22"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25" t="s">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25" t="s">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="25"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25" t="s">
+      <c r="E44" s="16"/>
+      <c r="F44" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="25"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="28" t="s">
+      <c r="D48" s="18"/>
+      <c r="E48" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -3752,6 +3757,48 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:E4"/>
@@ -3765,48 +3812,6 @@
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FORMATO DE ITEMS BORRADOS Y ANULADOS
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="140">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t>Generacion de Notas de Credito.</t>
+  </si>
+  <si>
+    <t>Formato de items borrados y anulados</t>
   </si>
 </sst>
 </file>
@@ -640,27 +643,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -678,6 +660,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1336,7 +1339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -1351,32 +1354,32 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1390,13 +1393,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1822,11 +1825,16 @@
       <c r="B38" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C38" s="14"/>
+      <c r="C38" s="14" t="s">
+        <v>139</v>
+      </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
+      <c r="H38" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
@@ -1927,94 +1935,94 @@
       <c r="G48" s="8"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22" t="s">
+      <c r="C51" s="24"/>
+      <c r="D51" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22" t="s">
+      <c r="E51" s="24"/>
+      <c r="F51" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="22"/>
+      <c r="G51" s="24"/>
     </row>
     <row r="52" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20" t="s">
+      <c r="C52" s="22"/>
+      <c r="D52" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20" t="s">
+      <c r="E52" s="22"/>
+      <c r="F52" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="20"/>
+      <c r="G52" s="22"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16" t="s">
+      <c r="C53" s="25"/>
+      <c r="D53" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16" t="s">
+      <c r="E53" s="25"/>
+      <c r="F53" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="16"/>
+      <c r="G53" s="25"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16" t="s">
+      <c r="C54" s="25"/>
+      <c r="D54" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16" t="s">
+      <c r="E54" s="25"/>
+      <c r="F54" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G54" s="16"/>
+      <c r="G54" s="25"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="17"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
     </row>
     <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="18" t="s">
+      <c r="C58" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D58" s="18"/>
-      <c r="E58" s="19" t="s">
+      <c r="D58" s="27"/>
+      <c r="E58" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
@@ -2034,35 +2042,26 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
@@ -2079,26 +2078,35 @@
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2113,7 +2121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C22" sqref="C22:G22"/>
     </sheetView>
   </sheetViews>
@@ -2127,29 +2135,29 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="29" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
-      <c r="F3" s="28"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -2166,13 +2174,13 @@
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -2512,92 +2520,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22" t="s">
+      <c r="C41" s="24"/>
+      <c r="D41" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22" t="s">
+      <c r="E41" s="24"/>
+      <c r="F41" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="22"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20" t="s">
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="20"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16" t="s">
+      <c r="E43" s="25"/>
+      <c r="F43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="25"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16" t="s">
+      <c r="C44" s="25"/>
+      <c r="D44" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="16"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19" t="s">
+      <c r="D48" s="27"/>
+      <c r="E48" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -2617,6 +2625,48 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -2630,48 +2680,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2699,29 +2707,29 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="29" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
-      <c r="F3" s="28"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -2738,13 +2746,13 @@
       <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -3056,92 +3064,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22" t="s">
+      <c r="C41" s="24"/>
+      <c r="D41" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22" t="s">
+      <c r="E41" s="24"/>
+      <c r="F41" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="22"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20" t="s">
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="20"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16" t="s">
+      <c r="E43" s="25"/>
+      <c r="F43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="25"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16" t="s">
+      <c r="C44" s="25"/>
+      <c r="D44" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="16"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19" t="s">
+      <c r="D48" s="27"/>
+      <c r="E48" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -3161,6 +3169,48 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3174,48 +3224,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -3244,32 +3252,32 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="15"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
@@ -3283,13 +3291,13 @@
       <c r="B7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="12" t="s">
         <v>87</v>
       </c>
@@ -3652,92 +3660,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22" t="s">
+      <c r="C41" s="24"/>
+      <c r="D41" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22" t="s">
+      <c r="E41" s="24"/>
+      <c r="F41" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="22"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20" t="s">
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G42" s="20"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16" t="s">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16" t="s">
+      <c r="E43" s="25"/>
+      <c r="F43" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="25"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16" t="s">
+      <c r="C44" s="25"/>
+      <c r="D44" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="G44" s="16"/>
+      <c r="G44" s="25"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="19" t="s">
+      <c r="D48" s="27"/>
+      <c r="E48" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -3757,6 +3765,48 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -3770,48 +3820,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CCFN-A035-A01 ASIGNACION DE ENVIOS POR RUTA
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="156">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>Rafael / Joaquin</t>
+  </si>
+  <si>
+    <t>Asignacion de envios por ruta</t>
   </si>
 </sst>
 </file>
@@ -1493,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:G42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,11 +2042,16 @@
       <c r="B42" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="16"/>
+      <c r="C42" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
+      <c r="H42" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">

</xml_diff>

<commit_message>
MOVIMIENTOS INTERNOS DE PRODUCCION E INVENTARIOS PARA AUXILIARES DE PANADERIA
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="D-FORMATOS" sheetId="4" r:id="rId4"/>
     <sheet name="E-ACTAS DE CAPACITACION" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="158">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -544,6 +544,12 @@
   </si>
   <si>
     <t>Asignacion de envios por ruta</t>
+  </si>
+  <si>
+    <t>Rafael Castañeda</t>
+  </si>
+  <si>
+    <t>Movimientos internos de produccion e inventario para auxiliares de panaderia</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
@@ -4015,8 +4021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4129,11 +4135,16 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>157</v>
+      </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
+      <c r="H11" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">

</xml_diff>

<commit_message>
CCFN-B020-A01-F008-R00 Manual de usuario Surtido de RT de salida
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
     <sheet name="B-MANUAL USUARIO" sheetId="2" r:id="rId2"/>
     <sheet name="C-MANUAL SOPORTE" sheetId="3" r:id="rId3"/>
-    <sheet name="D-FORMATOS" sheetId="4" r:id="rId4"/>
-    <sheet name="E-ACTAS DE CAPACITACION" sheetId="5" r:id="rId5"/>
+    <sheet name="E-ACTAS DE CAPACITACION" sheetId="5" r:id="rId4"/>
+    <sheet name="D-FORMATOS" sheetId="4" r:id="rId5"/>
+    <sheet name="F-ACTA DE REUNION" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="168">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -550,6 +551,36 @@
   </si>
   <si>
     <t>Movimientos internos de produccion e inventario para auxiliares de panaderia</t>
+  </si>
+  <si>
+    <t>Conversión de pedido de venta a factura.</t>
+  </si>
+  <si>
+    <t>Configuración cuenta de Outlook</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NOMBRE ACTA DE REUNION.</t>
+  </si>
+  <si>
+    <t>SECUENCIA ACTA DE REUNION</t>
+  </si>
+  <si>
+    <t>Call Center</t>
+  </si>
+  <si>
+    <t>Tarimas centro de distrubucion</t>
+  </si>
+  <si>
+    <t>Renovacion de pedidos de compra y centro de distribucion</t>
+  </si>
+  <si>
+    <t>Propuestas para integrar en cambio de punto de venta</t>
+  </si>
+  <si>
+    <t>Presentacion final de cubo</t>
+  </si>
+  <si>
+    <t>Surtido de RT de salida</t>
   </si>
 </sst>
 </file>
@@ -675,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -709,6 +740,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1237,6 +1274,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2" descr="Resultado de imagen para comercial de carnes frias del norte sa de cv"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="466725" y="276225"/>
+          <a:ext cx="952500" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>669925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="logoservlet"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" r:link="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4581525" y="219075"/>
+          <a:ext cx="555625" cy="512445"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1517,36 +1647,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -1556,13 +1686,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="12" t="s">
         <v>80</v>
       </c>
@@ -1571,13 +1701,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>84</v>
       </c>
@@ -1586,13 +1716,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>87</v>
       </c>
@@ -1601,13 +1731,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>86</v>
       </c>
@@ -1616,13 +1746,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>86</v>
       </c>
@@ -1631,13 +1761,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>84</v>
       </c>
@@ -1646,13 +1776,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>87</v>
       </c>
@@ -1661,37 +1791,37 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
       <c r="H16" t="s">
         <v>88</v>
       </c>
@@ -1700,97 +1830,97 @@
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" t="s">
         <v>89</v>
       </c>
@@ -1799,25 +1929,25 @@
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
       <c r="H26" t="s">
         <v>86</v>
       </c>
@@ -1826,25 +1956,25 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" t="s">
         <v>87</v>
       </c>
@@ -1853,13 +1983,13 @@
       <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" t="s">
         <v>87</v>
       </c>
@@ -1868,13 +1998,13 @@
       <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" t="s">
         <v>86</v>
       </c>
@@ -1883,13 +2013,13 @@
       <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
       <c r="H31" t="s">
         <v>87</v>
       </c>
@@ -1898,13 +2028,13 @@
       <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
       <c r="H32" t="s">
         <v>87</v>
       </c>
@@ -1913,13 +2043,13 @@
       <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
       <c r="H33" t="s">
         <v>109</v>
       </c>
@@ -1928,13 +2058,13 @@
       <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
       <c r="H34" t="s">
         <v>111</v>
       </c>
@@ -1943,13 +2073,13 @@
       <c r="B35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
       <c r="H35" t="s">
         <v>86</v>
       </c>
@@ -1958,13 +2088,13 @@
       <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
       <c r="H36" t="s">
         <v>117</v>
       </c>
@@ -1973,13 +2103,13 @@
       <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
       <c r="H37" t="s">
         <v>87</v>
       </c>
@@ -1988,13 +2118,13 @@
       <c r="B38" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
       <c r="H38" t="s">
         <v>87</v>
       </c>
@@ -2003,13 +2133,13 @@
       <c r="B39" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
       <c r="H39" t="s">
         <v>87</v>
       </c>
@@ -2018,13 +2148,13 @@
       <c r="B40" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
       <c r="H40" t="s">
         <v>87</v>
       </c>
@@ -2033,13 +2163,13 @@
       <c r="B41" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
       <c r="H41" t="s">
         <v>154</v>
       </c>
@@ -2048,13 +2178,13 @@
       <c r="B42" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
       <c r="H42" t="s">
         <v>87</v>
       </c>
@@ -2063,51 +2193,51 @@
       <c r="B43" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="13"/>
@@ -2118,110 +2248,110 @@
       <c r="G48" s="8"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26" t="s">
+      <c r="C51" s="28"/>
+      <c r="D51" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26" t="s">
+      <c r="E51" s="28"/>
+      <c r="F51" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="G51" s="26"/>
+      <c r="G51" s="28"/>
     </row>
     <row r="52" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24" t="s">
+      <c r="C52" s="26"/>
+      <c r="D52" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24" t="s">
+      <c r="E52" s="26"/>
+      <c r="F52" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="24"/>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27" t="s">
+      <c r="C53" s="29"/>
+      <c r="D53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27" t="s">
+      <c r="E53" s="29"/>
+      <c r="F53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G53" s="27"/>
+      <c r="G53" s="29"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27" t="s">
+      <c r="C54" s="29"/>
+      <c r="D54" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27" t="s">
+      <c r="E54" s="29"/>
+      <c r="F54" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G54" s="27"/>
+      <c r="G54" s="29"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="D58" s="28"/>
-      <c r="E58" s="29" t="s">
+      <c r="D58" s="30"/>
+      <c r="E58" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="65">
@@ -2304,8 +2434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:G47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,36 +2448,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2357,347 +2487,353 @@
       <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="C26" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="C27" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -2707,108 +2843,108 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="26"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="24"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27" t="s">
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27" t="s">
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29" t="s">
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -2880,8 +3016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,36 +3030,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -2933,315 +3069,315 @@
       <c r="B7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3251,108 +3387,108 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="26"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="24"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27" t="s">
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27" t="s">
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29" t="s">
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -3425,6 +3561,572 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B47" sqref="B47:G47"/>
     </sheetView>
   </sheetViews>
@@ -3439,36 +4141,36 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -3478,13 +4180,13 @@
       <c r="B7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="12" t="s">
         <v>80</v>
       </c>
@@ -3493,13 +4195,13 @@
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
       <c r="H8" t="s">
         <v>81</v>
       </c>
@@ -3508,13 +4210,13 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
       <c r="H9" t="s">
         <v>81</v>
       </c>
@@ -3523,13 +4225,13 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
       <c r="H10" t="s">
         <v>81</v>
       </c>
@@ -3538,13 +4240,13 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
       <c r="H11" t="s">
         <v>81</v>
       </c>
@@ -3553,13 +4255,13 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
       <c r="H12" t="s">
         <v>82</v>
       </c>
@@ -3568,13 +4270,13 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
       <c r="H13" t="s">
         <v>83</v>
       </c>
@@ -3583,13 +4285,13 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" t="s">
         <v>81</v>
       </c>
@@ -3598,13 +4300,13 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
       <c r="H15" t="s">
         <v>81</v>
       </c>
@@ -3613,231 +4315,231 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -3847,108 +4549,108 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="26"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="24"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27" t="s">
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27" t="s">
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29" t="s">
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -4017,394 +4719,380 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:G12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="15" t="s">
+      <c r="B4" s="22"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H5" s="1"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="12" t="s">
-        <v>136</v>
-      </c>
+      <c r="B7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" t="s">
-        <v>139</v>
-      </c>
+      <c r="C8" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
+      <c r="C9" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" t="s">
-        <v>142</v>
-      </c>
+      <c r="C10" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" t="s">
-        <v>156</v>
-      </c>
+      <c r="C11" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="C12" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
@@ -4414,111 +5102,153 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="G42" s="24"/>
-    </row>
-    <row r="43" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="27" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27" t="s">
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="27"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27" t="s">
+      <c r="B44" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27" t="s">
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="27"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29" t="s">
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="B43:C43"/>
@@ -4532,48 +5262,6 @@
     <mergeCell ref="E48:G48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Acta de reunion PDV BNEXT menudeo, mayoreo
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
     <sheet name="B-MANUAL USUARIO" sheetId="2" r:id="rId2"/>
     <sheet name="C-MANUAL SOPORTE" sheetId="3" r:id="rId3"/>
-    <sheet name="E-ACTAS DE CAPACITACION" sheetId="5" r:id="rId4"/>
-    <sheet name="D-FORMATOS" sheetId="4" r:id="rId5"/>
+    <sheet name="D-FORMATOS" sheetId="4" r:id="rId4"/>
+    <sheet name="E-ACTAS DE CAPACITACION" sheetId="5" r:id="rId5"/>
     <sheet name="F-ACTA DE REUNION" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="170">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t>Surtido de RT de salida</t>
+  </si>
+  <si>
+    <t>Prueba de PDV BNEXT menudeo</t>
+  </si>
+  <si>
+    <t>Prueba de PDV BNEXT mayoreo</t>
   </si>
 </sst>
 </file>
@@ -2434,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3561,573 +3567,7 @@
   <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:G47"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4719,12 +4159,578 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4848,7 +4854,9 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="18" t="s">
+        <v>168</v>
+      </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -4858,7 +4866,9 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="18" t="s">
+        <v>169</v>
+      </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>

</xml_diff>

<commit_message>
ANEXO MANUAL DE USUARIO
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="171">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -508,12 +508,6 @@
     <t>Erika Gone</t>
   </si>
   <si>
-    <t>Capacitacion de induccion de Protheus (Stock/Costos-Compras).</t>
-  </si>
-  <si>
-    <t>Capacitacion de induccion de Protheus (Compras).</t>
-  </si>
-  <si>
     <t>ELABORÓ</t>
   </si>
   <si>
@@ -587,6 +581,15 @@
   </si>
   <si>
     <t>Prueba de PDV BNEXT mayoreo</t>
+  </si>
+  <si>
+    <t>Introduccion a sistemas</t>
+  </si>
+  <si>
+    <t>Pendientes po realizar 3.3, contact center y PDV</t>
+  </si>
+  <si>
+    <t>Alta de cuenta de cheques en catalogo de bancos</t>
   </si>
 </sst>
 </file>
@@ -759,6 +762,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,24 +797,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1653,32 +1656,32 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1692,13 +1695,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
       <c r="H7" s="12" t="s">
         <v>80</v>
       </c>
@@ -2170,14 +2173,14 @@
         <v>121</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
       <c r="H41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -2185,7 +2188,7 @@
         <v>122</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -2254,94 +2257,94 @@
       <c r="G48" s="8"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="27" t="s">
+      <c r="B50" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28" t="s">
+      <c r="G51" s="25"/>
+    </row>
+    <row r="52" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="G51" s="28"/>
-    </row>
-    <row r="52" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26" t="s">
+      <c r="C52" s="24"/>
+      <c r="D52" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="26"/>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29" t="s">
+      <c r="C53" s="20"/>
+      <c r="D53" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29" t="s">
+      <c r="E53" s="20"/>
+      <c r="F53" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G53" s="29"/>
+      <c r="G53" s="20"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29" t="s">
+      <c r="C54" s="20"/>
+      <c r="D54" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29" t="s">
+      <c r="E54" s="20"/>
+      <c r="F54" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G54" s="29"/>
+      <c r="G54" s="20"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
     </row>
     <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C58" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D58" s="30"/>
-      <c r="E58" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="22"/>
+      <c r="E58" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
@@ -2361,26 +2364,35 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
@@ -2397,35 +2409,26 @@
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2440,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,29 +2457,29 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
-      <c r="F3" s="25"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
@@ -2493,13 +2496,13 @@
       <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -2710,7 +2713,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
@@ -2722,7 +2725,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -2734,7 +2737,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
@@ -2745,7 +2748,9 @@
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
@@ -2849,92 +2854,1794 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="28"/>
+      <c r="G41" s="25"/>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26" t="s">
+      <c r="B42" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="26"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
+      <c r="C43" s="20"/>
+      <c r="D43" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29" t="s">
+      <c r="E43" s="20"/>
+      <c r="F43" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="29"/>
+      <c r="G43" s="20"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
+      <c r="C44" s="20"/>
+      <c r="D44" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="29"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="26"/>
+      <c r="C2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="28"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="26"/>
+      <c r="C2" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="28"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="26"/>
+      <c r="C2" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="28"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="22"/>
+      <c r="E48" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -3018,12 +4725,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,33 +4743,33 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="32" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
-      <c r="F3" s="25"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="19"/>
@@ -3075,20 +4782,20 @@
       <c r="B7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
+      <c r="C7" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -3099,7 +4806,9 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="18" t="s">
+        <v>161</v>
+      </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
@@ -3109,7 +4818,9 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="18" t="s">
+        <v>162</v>
+      </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
@@ -3119,7 +4830,9 @@
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="18" t="s">
+        <v>163</v>
+      </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
@@ -3129,7 +4842,9 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="18" t="s">
+        <v>164</v>
+      </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -3139,7 +4854,9 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -3149,7 +4866,9 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="18" t="s">
+        <v>167</v>
+      </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -3159,7 +4878,9 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="18" t="s">
+        <v>169</v>
+      </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
@@ -3393,1255 +5114,92 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
+      <c r="G41" s="25"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="24"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
+      <c r="D48" s="22"/>
+      <c r="E48" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H50"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -4723,560 +5281,4 @@
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H5" s="1"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G41" s="28"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G44" s="29"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="E49:G49"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
-  </ignoredErrors>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Proceso de anticipo version 3.3 CFDI
</commit_message>
<xml_diff>
--- a/099. SECUENCIA DE DOCUMENTACION.xlsx
+++ b/099. SECUENCIA DE DOCUMENTACION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="A-PROYECTOS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="174">
   <si>
     <t>SECUENCIA DE PROYECTOS</t>
   </si>
@@ -590,6 +590,15 @@
   </si>
   <si>
     <t>Alta de cuenta de cheques en catalogo de bancos</t>
+  </si>
+  <si>
+    <t>Joaquin Gallardo</t>
+  </si>
+  <si>
+    <t>Envio Electronico recibo de pago a clientes</t>
+  </si>
+  <si>
+    <t>Proceso de anticipo version 3.3 CFDI</t>
   </si>
 </sst>
 </file>
@@ -762,24 +771,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,6 +788,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1641,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,32 +1665,32 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1695,13 +1704,13 @@
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="12" t="s">
         <v>80</v>
       </c>
@@ -2202,21 +2211,31 @@
       <c r="B43" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="18"/>
+      <c r="C43" s="18" t="s">
+        <v>172</v>
+      </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="18"/>
+      <c r="H43" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C44" s="18"/>
+      <c r="C44" s="18" t="s">
+        <v>173</v>
+      </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
+      <c r="H44" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
@@ -2257,94 +2276,94 @@
       <c r="G48" s="8"/>
     </row>
     <row r="50" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="21" t="s">
+      <c r="B50" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25" t="s">
+      <c r="C51" s="28"/>
+      <c r="D51" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25" t="s">
+      <c r="E51" s="28"/>
+      <c r="F51" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="G51" s="25"/>
+      <c r="G51" s="28"/>
     </row>
     <row r="52" spans="2:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24" t="s">
+      <c r="C52" s="26"/>
+      <c r="D52" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24" t="s">
+      <c r="E52" s="26"/>
+      <c r="F52" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="24"/>
+      <c r="G52" s="26"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20" t="s">
+      <c r="C53" s="29"/>
+      <c r="D53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20" t="s">
+      <c r="E53" s="29"/>
+      <c r="F53" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G53" s="20"/>
+      <c r="G53" s="29"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20" t="s">
+      <c r="C54" s="29"/>
+      <c r="D54" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20" t="s">
+      <c r="E54" s="29"/>
+      <c r="F54" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G54" s="20"/>
+      <c r="G54" s="29"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
     </row>
     <row r="58" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="23" t="s">
+      <c r="D58" s="30"/>
+      <c r="E58" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
@@ -2364,35 +2383,26 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C2:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E59:G59"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
@@ -2409,26 +2419,35 @@
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="C29:G29"/>
     <mergeCell ref="C30:G30"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2443,7 +2462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29:G29"/>
     </sheetView>
   </sheetViews>
@@ -2457,29 +2476,29 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
-      <c r="F3" s="31"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="19"/>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="28"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
@@ -2496,13 +2515,13 @@
       <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
@@ -2854,92 +2873,1799 @@
       <c r="G38" s="8"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25" t="s">
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25" t="s">
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="G41" s="25"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G42" s="24"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20" t="s">
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G43" s="20"/>
+      <c r="G43" s="29"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20" t="s">
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20" t="s">
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="20"/>
+      <c r="G44" s="29"/>
     </row>
     <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C48" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="23" t="s">
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="23"/>
-      <c r="G48" s="23"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" s="26"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="29"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="29"/>
+    </row>
+    <row r="47" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D48" s="30"/>
+      <c r="E48" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="7"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="7"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="55">
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:G49"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B8:B37" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14"